<commit_message>
Functional Create_DoEs.py and Optimal_Design.R with readme and guide
Fix small issues with Create_DoEs.py (mainly due to incompatibility of dexpy with pandas >2.0) and Optimal_Design.R (fixed auto-adding of experiments). Also add proper ReadMe.md and a guide in docs.
</commit_message>
<xml_diff>
--- a/src/Features.xlsx
+++ b/src/Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc\Atmonia Dropbox\Marc Francis Hidalgo\Scripts\How to DoE and ML\DoE\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF4B9F8-94BA-4A15-B674-EE26C0999518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC84BC18-A6B0-44D0-B338-B42E01551B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1964EAFC-59E3-41C7-9D0F-144AE69FFC35}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1964EAFC-59E3-41C7-9D0F-144AE69FFC35}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuous" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Feature</t>
   </si>
@@ -48,37 +48,7 @@
     <t>Max Level</t>
   </si>
   <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Cation</t>
-  </si>
-  <si>
-    <t>Li</t>
-  </si>
-  <si>
-    <t>Na</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>Levels</t>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>N2</t>
-  </si>
-  <si>
-    <t>Ar</t>
   </si>
 </sst>
 </file>
@@ -122,10 +92,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -134,13 +113,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -480,60 +466,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F485943-2C44-4AA4-93FE-630A947A0394}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="15.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="15.26953125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -544,58 +498,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15987C72-CEF5-41FB-AB31-CAD6186BCF03}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="18.81640625" style="4" customWidth="1"/>
     <col min="12" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
+      <c r="B1" s="7" t="s">
+        <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>